<commit_message>
Separate sha2_end_to_end.py. Delete several files. Minor fixes
</commit_message>
<xml_diff>
--- a/docs/sha2_attack_stats.xlsx
+++ b/docs/sha2_attack_stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaaco\Documents\FortifyIQ\Github\sha2-attack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9695EF-5ECD-4B26-90F6-B158E9E7CB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645CAB68-E0DD-495E-94A3-AB77E10BD3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F46EC8F-B1BA-49E3-B4D3-5A58024BD9E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{5F46EC8F-B1BA-49E3-B4D3-5A58024BD9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="lsb" sheetId="1" r:id="rId1"/>
-    <sheet name="chart" sheetId="3" r:id="rId2"/>
-    <sheet name="res" sheetId="2" r:id="rId3"/>
+    <sheet name="res" sheetId="2" r:id="rId2"/>
+    <sheet name="chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -214,7 +214,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -242,6 +241,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,28 +368,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.765625E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8125</c:v>
+                  <c:v>6.15234375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.9375</c:v>
+                  <c:v>40.0390625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69.53125</c:v>
+                  <c:v>66.40625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.890625</c:v>
+                  <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>94.921875</c:v>
+                  <c:v>91.9921875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.4375</c:v>
+                  <c:v>96.38671875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>99.21875</c:v>
+                  <c:v>98.33984375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,22 +474,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1015625</c:v>
+                  <c:v>4.8828125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.7890625</c:v>
+                  <c:v>33.69140625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65.234375</c:v>
+                  <c:v>63.28125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.203125</c:v>
+                  <c:v>82.6171875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.53125</c:v>
+                  <c:v>91.11328125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94.53125</c:v>
+                  <c:v>96.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,9 +567,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -576,19 +574,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78125</c:v>
+                  <c:v>0.5859375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.3125</c:v>
+                  <c:v>21.09375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.25</c:v>
+                  <c:v>53.22265625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81.25</c:v>
+                  <c:v>76.3671875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.71875</c:v>
+                  <c:v>89.0625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,26 +664,20 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>9.765625E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.34375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.875</c:v>
+                  <c:v>28.80859375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.15625</c:v>
+                  <c:v>61.1328125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,12 +753,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
@@ -774,7 +760,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.90625</c:v>
+                  <c:v>2.5390625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +1982,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2004,17 +1990,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -2052,13 +2038,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>3.57818603515625</v>
       </c>
       <c r="D3" s="9">
@@ -2087,285 +2073,255 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="12">
-        <v>1.708984375</v>
-      </c>
-      <c r="D4" s="12">
-        <v>3.4759521484375</v>
-      </c>
-      <c r="E4" s="12">
-        <v>7.269287109375</v>
-      </c>
-      <c r="F4" s="12">
-        <v>18.8018798828125</v>
-      </c>
-      <c r="G4" s="12">
-        <v>48.8525390625</v>
-      </c>
-      <c r="H4" s="12">
-        <v>75.01220703125</v>
-      </c>
-      <c r="I4" s="12">
-        <v>88.00048828125</v>
-      </c>
-      <c r="J4" s="12">
-        <v>96.25244140625</v>
-      </c>
-      <c r="K4" s="13">
-        <v>95.95947265625</v>
+      <c r="C4" s="11"/>
+      <c r="D4" s="25">
+        <v>3.4393310546875</v>
+      </c>
+      <c r="E4" s="25">
+        <v>7.36236572265625</v>
+      </c>
+      <c r="F4" s="25">
+        <v>20.2743530273437</v>
+      </c>
+      <c r="G4" s="25">
+        <v>48.4344482421875</v>
+      </c>
+      <c r="H4" s="25">
+        <v>72.9949951171875</v>
+      </c>
+      <c r="I4" s="25">
+        <v>87.532043457031193</v>
+      </c>
+      <c r="J4" s="25">
+        <v>93.7225341796875</v>
+      </c>
+      <c r="K4" s="12">
+        <v>97.773742675781193</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3">
         <v>8</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12">
-        <v>1.38092041015625</v>
-      </c>
-      <c r="E5" s="12">
-        <v>2.7252197265625</v>
-      </c>
-      <c r="F5" s="12">
-        <v>5.548095703125</v>
-      </c>
-      <c r="G5" s="12">
-        <v>13.0218505859375</v>
-      </c>
-      <c r="H5" s="12">
-        <v>36.785888671875</v>
-      </c>
-      <c r="I5" s="12">
-        <v>68.1396484375</v>
-      </c>
-      <c r="J5" s="12">
-        <v>86.5234375</v>
-      </c>
-      <c r="K5" s="13">
-        <v>90.52734375</v>
+      <c r="C5" s="11"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25">
+        <v>2.72674560546875</v>
+      </c>
+      <c r="F5" s="25">
+        <v>5.59539794921875</v>
+      </c>
+      <c r="G5" s="25">
+        <v>12.4481201171875</v>
+      </c>
+      <c r="H5" s="25">
+        <v>37.200927734375</v>
+      </c>
+      <c r="I5" s="25">
+        <v>65.238952636718693</v>
+      </c>
+      <c r="J5" s="25">
+        <v>83.033752441406193</v>
+      </c>
+      <c r="K5" s="12">
+        <v>92.1905517578125</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <v>16</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12">
-        <v>0.70037841796875</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1.4617919921875</v>
-      </c>
-      <c r="G6" s="12">
-        <v>2.9876708984375</v>
-      </c>
-      <c r="H6" s="12">
-        <v>6.70166015625</v>
-      </c>
-      <c r="I6" s="12">
-        <v>17.2607421875</v>
-      </c>
-      <c r="J6" s="12">
-        <v>40.13671875</v>
-      </c>
-      <c r="K6" s="13">
-        <v>72.705078125</v>
+      <c r="C6" s="11"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25">
+        <v>3.06396484375</v>
+      </c>
+      <c r="H6" s="25">
+        <v>6.585693359375</v>
+      </c>
+      <c r="I6" s="25">
+        <v>16.3375854492187</v>
+      </c>
+      <c r="J6" s="25">
+        <v>45.0119018554687</v>
+      </c>
+      <c r="K6" s="12">
+        <v>70.9197998046875</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3">
         <v>32</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12">
-        <v>0.78125</v>
-      </c>
-      <c r="H7" s="12">
-        <v>1.708984375</v>
-      </c>
-      <c r="I7" s="12">
-        <v>3.411865234375</v>
-      </c>
-      <c r="J7" s="12">
-        <v>6.4208984375</v>
-      </c>
-      <c r="K7" s="13">
-        <v>18.24951171875</v>
+      <c r="C7" s="11"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25">
+        <v>3.33099365234375</v>
+      </c>
+      <c r="J7" s="25">
+        <v>6.866455078125</v>
+      </c>
+      <c r="K7" s="12">
+        <v>16.6427612304687</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7">
         <v>64</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15">
-        <v>0.732421875</v>
-      </c>
-      <c r="J8" s="15">
-        <v>1.6845703125</v>
-      </c>
-      <c r="K8" s="16">
-        <v>3.35693359375</v>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15">
+        <v>3.28369140625</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="12">
-        <v>0.873565673828125</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1.7509460449218699</v>
-      </c>
-      <c r="E9" s="12">
-        <v>3.63922119140625</v>
-      </c>
-      <c r="F9" s="12">
-        <v>9.07135009765625</v>
-      </c>
-      <c r="G9" s="12">
-        <v>24.249267578125</v>
-      </c>
-      <c r="H9" s="12">
-        <v>53.369140625</v>
-      </c>
-      <c r="I9" s="12">
-        <v>72.9583740234375</v>
-      </c>
-      <c r="J9" s="12">
-        <v>87.518310546875</v>
-      </c>
-      <c r="K9" s="13">
-        <v>91.2109375</v>
+      <c r="C9" s="11"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25">
+        <v>3.59344482421875</v>
+      </c>
+      <c r="F9" s="25">
+        <v>9.02862548828125</v>
+      </c>
+      <c r="G9" s="25">
+        <v>24.6826171875</v>
+      </c>
+      <c r="H9" s="25">
+        <v>53.771209716796797</v>
+      </c>
+      <c r="I9" s="25">
+        <v>74.427795410156193</v>
+      </c>
+      <c r="J9" s="25">
+        <v>86.533355712890597</v>
+      </c>
+      <c r="K9" s="12">
+        <v>93.013000488281193</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12">
-        <v>2.2621154785156201</v>
-      </c>
-      <c r="F10" s="12">
-        <v>5.1055908203125</v>
-      </c>
-      <c r="G10" s="12">
-        <v>12.4588012695312</v>
-      </c>
-      <c r="H10" s="12">
-        <v>31.9915771484375</v>
-      </c>
-      <c r="I10" s="12">
-        <v>56.6253662109375</v>
-      </c>
-      <c r="J10" s="12">
-        <v>77.18505859375</v>
-      </c>
-      <c r="K10" s="13">
-        <v>89.48974609375</v>
+      <c r="C10" s="11"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25">
+        <v>2.33917236328125</v>
+      </c>
+      <c r="F10" s="25">
+        <v>5.2009582519531197</v>
+      </c>
+      <c r="G10" s="25">
+        <v>13.7718200683593</v>
+      </c>
+      <c r="H10" s="25">
+        <v>35.286712646484297</v>
+      </c>
+      <c r="I10" s="25">
+        <v>59.9166870117187</v>
+      </c>
+      <c r="J10" s="25">
+        <v>78.954315185546804</v>
+      </c>
+      <c r="K10" s="12">
+        <v>89.262390136718693</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12">
-        <v>1.16729736328125</v>
-      </c>
-      <c r="F11" s="12">
-        <v>2.17742919921875</v>
-      </c>
-      <c r="G11" s="12">
-        <v>5.0933837890625</v>
-      </c>
-      <c r="H11" s="12">
-        <v>11.6943359375</v>
-      </c>
-      <c r="I11" s="12">
-        <v>31.3446044921875</v>
-      </c>
-      <c r="J11" s="12">
-        <v>59.185791015625</v>
-      </c>
-      <c r="K11" s="13">
-        <v>80.11474609375</v>
+      <c r="C11" s="11"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25">
+        <v>2.33001708984375</v>
+      </c>
+      <c r="G11" s="25">
+        <v>4.83245849609375</v>
+      </c>
+      <c r="H11" s="25">
+        <v>13.0393981933593</v>
+      </c>
+      <c r="I11" s="25">
+        <v>32.8277587890625</v>
+      </c>
+      <c r="J11" s="25">
+        <v>59.343719482421797</v>
+      </c>
+      <c r="K11" s="12">
+        <v>78.411865234375</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="3">
         <v>16</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12">
-        <v>0.77667236328125</v>
-      </c>
-      <c r="G12" s="12">
-        <v>1.4801025390625</v>
-      </c>
-      <c r="H12" s="12">
-        <v>2.8350830078125</v>
-      </c>
-      <c r="I12" s="12">
-        <v>8.184814453125</v>
-      </c>
-      <c r="J12" s="12">
-        <v>17.767333984375</v>
-      </c>
-      <c r="K12" s="13">
-        <v>41.937255859375</v>
+      <c r="C12" s="11"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25">
+        <v>3.0891418457031201</v>
+      </c>
+      <c r="I12" s="25">
+        <v>6.9831848144531197</v>
+      </c>
+      <c r="J12" s="25">
+        <v>19.7921752929687</v>
+      </c>
+      <c r="K12" s="12">
+        <v>45.351409912109297</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="6">
         <v>32</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17">
-        <v>0.823974609375</v>
-      </c>
-      <c r="I13" s="17">
-        <v>1.7120361328125</v>
-      </c>
-      <c r="J13" s="17">
-        <v>2.8076171875</v>
-      </c>
-      <c r="K13" s="18">
-        <v>7.6904296875</v>
+      <c r="C13" s="26"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16">
+        <v>3.1745910644531201</v>
+      </c>
+      <c r="K13" s="17">
+        <v>7.6423645019531197</v>
       </c>
     </row>
   </sheetData>
@@ -2388,7 +2344,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2396,17 +2352,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -2444,7 +2400,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
@@ -2454,309 +2410,279 @@
         <v>0</v>
       </c>
       <c r="D3" s="9">
-        <v>0</v>
+        <v>9.765625E-2</v>
       </c>
       <c r="E3" s="9">
-        <v>7.8125</v>
+        <v>6.15234375</v>
       </c>
       <c r="F3" s="9">
-        <v>35.9375</v>
+        <v>40.0390625</v>
       </c>
       <c r="G3" s="9">
-        <v>69.53125</v>
+        <v>66.40625</v>
       </c>
       <c r="H3" s="9">
-        <v>87.890625</v>
+        <v>87.5</v>
       </c>
       <c r="I3" s="9">
-        <v>94.921875</v>
+        <v>91.9921875</v>
       </c>
       <c r="J3" s="9">
-        <v>98.4375</v>
+        <v>96.38671875</v>
       </c>
       <c r="K3" s="10">
-        <v>99.21875</v>
+        <v>98.33984375</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="11"/>
+      <c r="D4" s="25">
         <v>0</v>
       </c>
-      <c r="D4" s="12">
+      <c r="E4" s="25">
         <v>0</v>
       </c>
-      <c r="E4" s="12">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12">
-        <v>4.1015625</v>
-      </c>
-      <c r="G4" s="12">
-        <v>33.7890625</v>
-      </c>
-      <c r="H4" s="12">
-        <v>65.234375</v>
-      </c>
-      <c r="I4" s="12">
-        <v>83.203125</v>
-      </c>
-      <c r="J4" s="12">
-        <v>94.53125</v>
-      </c>
-      <c r="K4" s="13">
-        <v>94.53125</v>
+      <c r="F4" s="25">
+        <v>4.8828125</v>
+      </c>
+      <c r="G4" s="25">
+        <v>33.69140625</v>
+      </c>
+      <c r="H4" s="25">
+        <v>63.28125</v>
+      </c>
+      <c r="I4" s="25">
+        <v>82.6171875</v>
+      </c>
+      <c r="J4" s="25">
+        <v>91.11328125</v>
+      </c>
+      <c r="K4" s="12">
+        <v>96.875</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="12">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25">
         <v>0</v>
       </c>
-      <c r="E5" s="12">
+      <c r="F5" s="25">
         <v>0</v>
       </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0.78125</v>
-      </c>
-      <c r="H5" s="12">
-        <v>20.3125</v>
-      </c>
-      <c r="I5" s="12">
-        <v>56.25</v>
-      </c>
-      <c r="J5" s="12">
-        <v>81.25</v>
-      </c>
-      <c r="K5" s="13">
-        <v>86.71875</v>
+      <c r="G5" s="25">
+        <v>0.5859375</v>
+      </c>
+      <c r="H5" s="25">
+        <v>21.09375</v>
+      </c>
+      <c r="I5" s="25">
+        <v>53.22265625</v>
+      </c>
+      <c r="J5" s="25">
+        <v>76.3671875</v>
+      </c>
+      <c r="K5" s="12">
+        <v>89.0625</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <v>16</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25">
         <v>0</v>
       </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="12">
+      <c r="H6" s="25">
+        <v>9.765625E-2</v>
+      </c>
+      <c r="I6" s="25">
         <v>2.34375</v>
       </c>
-      <c r="J6" s="12">
-        <v>21.875</v>
-      </c>
-      <c r="K6" s="13">
-        <v>60.15625</v>
+      <c r="J6" s="25">
+        <v>28.80859375</v>
+      </c>
+      <c r="K6" s="12">
+        <v>61.1328125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3">
         <v>32</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25">
         <v>0</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="25">
         <v>0</v>
       </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <v>0</v>
-      </c>
-      <c r="K7" s="13">
-        <v>3.90625</v>
+      <c r="K7" s="12">
+        <v>2.5390625</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7">
         <v>64</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0</v>
-      </c>
-      <c r="K8" s="16">
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25">
         <v>0</v>
       </c>
-      <c r="D9" s="12">
+      <c r="F9" s="25">
         <v>0</v>
       </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0.390625</v>
-      </c>
-      <c r="G9" s="12">
-        <v>9.375</v>
-      </c>
-      <c r="H9" s="12">
-        <v>39.0625</v>
-      </c>
-      <c r="I9" s="12">
-        <v>63.28125</v>
-      </c>
-      <c r="J9" s="12">
-        <v>82.8125</v>
-      </c>
-      <c r="K9" s="13">
-        <v>87.5</v>
+      <c r="G9" s="25">
+        <v>8.88671875</v>
+      </c>
+      <c r="H9" s="25">
+        <v>39.6484375</v>
+      </c>
+      <c r="I9" s="25">
+        <v>66.015625</v>
+      </c>
+      <c r="J9" s="25">
+        <v>81.93359375</v>
+      </c>
+      <c r="K9" s="12">
+        <v>90.4296875</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12">
+      <c r="C10" s="11"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25">
         <v>0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="25">
         <v>0</v>
       </c>
-      <c r="G10" s="12">
-        <v>0.9765625</v>
-      </c>
-      <c r="H10" s="12">
-        <v>14.453125</v>
-      </c>
-      <c r="I10" s="12">
-        <v>42.96875</v>
-      </c>
-      <c r="J10" s="12">
-        <v>70.3125</v>
-      </c>
-      <c r="K10" s="13">
-        <v>85.9375</v>
+      <c r="G10" s="25">
+        <v>1.171875</v>
+      </c>
+      <c r="H10" s="25">
+        <v>19.921875</v>
+      </c>
+      <c r="I10" s="25">
+        <v>47.8515625</v>
+      </c>
+      <c r="J10" s="25">
+        <v>71.875</v>
+      </c>
+      <c r="K10" s="12">
+        <v>85.3515625</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12">
+      <c r="C11" s="11"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25">
         <v>0</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="25">
         <v>0</v>
       </c>
-      <c r="G11" s="12">
-        <v>0</v>
-      </c>
-      <c r="H11" s="12">
-        <v>0</v>
-      </c>
-      <c r="I11" s="12">
-        <v>14.84375</v>
-      </c>
-      <c r="J11" s="12">
-        <v>47.65625</v>
-      </c>
-      <c r="K11" s="13">
-        <v>73.4375</v>
+      <c r="H11" s="25">
+        <v>0.68359375</v>
+      </c>
+      <c r="I11" s="25">
+        <v>15.625</v>
+      </c>
+      <c r="J11" s="25">
+        <v>46.38671875</v>
+      </c>
+      <c r="K11" s="12">
+        <v>70.80078125</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="3">
         <v>16</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12">
+      <c r="C12" s="11"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25">
         <v>0</v>
       </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="I12" s="25">
+        <v>9.765625E-2</v>
+      </c>
+      <c r="J12" s="25">
         <v>4.6875</v>
       </c>
-      <c r="K12" s="13">
-        <v>22.65625</v>
+      <c r="K12" s="12">
+        <v>29.8828125</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="6">
         <v>32</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17">
+      <c r="C13" s="26"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16">
         <v>0</v>
       </c>
-      <c r="I13" s="17">
-        <v>0</v>
-      </c>
-      <c r="J13" s="17">
-        <v>0</v>
-      </c>
-      <c r="K13" s="18">
+      <c r="K13" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor changes in the Excel
</commit_message>
<xml_diff>
--- a/docs/sha2_attack_stats.xlsx
+++ b/docs/sha2_attack_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaaco\Documents\FortifyIQ\Github\sha2-attack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645CAB68-E0DD-495E-94A3-AB77E10BD3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB4831B-EE60-42D1-BFE2-4498CB269E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{5F46EC8F-B1BA-49E3-B4D3-5A58024BD9E5}"/>
   </bookViews>
@@ -220,6 +220,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,8 +243,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,7 +799,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -812,8 +812,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
-                  <a:t># of traces</a:t>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t># of simulated SHA256 traces</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -831,7 +831,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -920,7 +920,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -933,9 +933,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Success ratio</a:t>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Success rate</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                  <a:t> (in %)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2800"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -952,7 +957,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1990,17 +1995,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -2038,7 +2043,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
@@ -2073,30 +2078,30 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3">
         <v>4</v>
       </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="25">
+      <c r="D4" s="18">
         <v>3.4393310546875</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="18">
         <v>7.36236572265625</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <v>20.2743530273437</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="18">
         <v>48.4344482421875</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="18">
         <v>72.9949951171875</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="18">
         <v>87.532043457031193</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="18">
         <v>93.7225341796875</v>
       </c>
       <c r="K4" s="12">
@@ -2104,28 +2109,28 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18">
         <v>2.72674560546875</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="18">
         <v>5.59539794921875</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="18">
         <v>12.4481201171875</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="18">
         <v>37.200927734375</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="18">
         <v>65.238952636718693</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="18">
         <v>83.033752441406193</v>
       </c>
       <c r="K5" s="12">
@@ -2133,24 +2138,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3">
         <v>16</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18">
         <v>3.06396484375</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="18">
         <v>6.585693359375</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="18">
         <v>16.3375854492187</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="18">
         <v>45.0119018554687</v>
       </c>
       <c r="K6" s="12">
@@ -2158,20 +2163,20 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3">
         <v>32</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18">
         <v>3.33099365234375</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="18">
         <v>6.866455078125</v>
       </c>
       <c r="K7" s="12">
@@ -2179,7 +2184,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="7">
         <v>64</v>
       </c>
@@ -2196,30 +2201,30 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18">
         <v>3.59344482421875</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="18">
         <v>9.02862548828125</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="18">
         <v>24.6826171875</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="18">
         <v>53.771209716796797</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="18">
         <v>74.427795410156193</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="18">
         <v>86.533355712890597</v>
       </c>
       <c r="K9" s="12">
@@ -2227,28 +2232,28 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3">
         <v>4</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18">
         <v>2.33917236328125</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="18">
         <v>5.2009582519531197</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="18">
         <v>13.7718200683593</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="18">
         <v>35.286712646484297</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="18">
         <v>59.9166870117187</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="18">
         <v>78.954315185546804</v>
       </c>
       <c r="K10" s="12">
@@ -2256,26 +2261,26 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18">
         <v>2.33001708984375</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="18">
         <v>4.83245849609375</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="18">
         <v>13.0393981933593</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="18">
         <v>32.8277587890625</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="18">
         <v>59.343719482421797</v>
       </c>
       <c r="K11" s="12">
@@ -2283,22 +2288,22 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3">
         <v>16</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
         <v>3.0891418457031201</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="18">
         <v>6.9831848144531197</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="18">
         <v>19.7921752929687</v>
       </c>
       <c r="K12" s="12">
@@ -2306,11 +2311,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="6">
         <v>32</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -2352,17 +2357,17 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -2400,7 +2405,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
@@ -2435,30 +2440,30 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3">
         <v>4</v>
       </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="25">
+      <c r="D4" s="18">
         <v>0</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="18">
         <v>0</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="18">
         <v>4.8828125</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="18">
         <v>33.69140625</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="18">
         <v>63.28125</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="18">
         <v>82.6171875</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="18">
         <v>91.11328125</v>
       </c>
       <c r="K4" s="12">
@@ -2466,28 +2471,28 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18">
         <v>0</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="18">
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="18">
         <v>0.5859375</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="18">
         <v>21.09375</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="18">
         <v>53.22265625</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="18">
         <v>76.3671875</v>
       </c>
       <c r="K5" s="12">
@@ -2495,24 +2500,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3">
         <v>16</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18">
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="18">
         <v>9.765625E-2</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="18">
         <v>2.34375</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="18">
         <v>28.80859375</v>
       </c>
       <c r="K6" s="12">
@@ -2520,20 +2525,20 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3">
         <v>32</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18">
         <v>0</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="18">
         <v>0</v>
       </c>
       <c r="K7" s="12">
@@ -2541,7 +2546,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="7">
         <v>64</v>
       </c>
@@ -2558,30 +2563,30 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18">
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="18">
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="18">
         <v>8.88671875</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="18">
         <v>39.6484375</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="18">
         <v>66.015625</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="18">
         <v>81.93359375</v>
       </c>
       <c r="K9" s="12">
@@ -2589,28 +2594,28 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3">
         <v>4</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18">
         <v>0</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="18">
         <v>0</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="18">
         <v>1.171875</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="18">
         <v>19.921875</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="18">
         <v>47.8515625</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="18">
         <v>71.875</v>
       </c>
       <c r="K10" s="12">
@@ -2618,26 +2623,26 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18">
         <v>0</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="18">
         <v>0</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="18">
         <v>0.68359375</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="18">
         <v>15.625</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="18">
         <v>46.38671875</v>
       </c>
       <c r="K11" s="12">
@@ -2645,22 +2650,22 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3">
         <v>16</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
         <v>0</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="18">
         <v>9.765625E-2</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="18">
         <v>4.6875</v>
       </c>
       <c r="K12" s="12">
@@ -2668,11 +2673,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="6">
         <v>32</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>

</xml_diff>